<commit_message>
added DE statement notes tab
</commit_message>
<xml_diff>
--- a/DE.xlsx
+++ b/DE.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32906c935fa0eb4f/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1692" documentId="8_{2959E65E-55D8-40F5-B350-6BD91C9C1EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C8DB9A6-0FE3-4648-9DA6-383997F9CC69}"/>
+  <xr:revisionPtr revIDLastSave="1768" documentId="8_{2959E65E-55D8-40F5-B350-6BD91C9C1EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57F8A797-0270-42B1-AB54-F904851851F4}"/>
   <bookViews>
-    <workbookView xWindow="20050" yWindow="560" windowWidth="17900" windowHeight="19850" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20050" yWindow="560" windowWidth="17900" windowHeight="19850" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Model" sheetId="7" r:id="rId2"/>
     <sheet name="ModelOLD" sheetId="2" r:id="rId3"/>
     <sheet name="Parts" sheetId="5" r:id="rId4"/>
-    <sheet name="Earnings Call Notes" sheetId="6" r:id="rId5"/>
+    <sheet name="Statement Notes" sheetId="6" r:id="rId5"/>
     <sheet name="Manufacturing" sheetId="3" r:id="rId6"/>
     <sheet name="IP" sheetId="4" r:id="rId7"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="255">
   <si>
     <t>Price</t>
   </si>
@@ -763,6 +763,81 @@
   <si>
     <t>Other Non-cash</t>
   </si>
+  <si>
+    <t>Lower shipping volumes, price offset</t>
+  </si>
+  <si>
+    <t>Small Ag &amp; Turf</t>
+  </si>
+  <si>
+    <t>Construction and Forestry</t>
+  </si>
+  <si>
+    <t>Sales and profit up, higher shipping volumes and price offset</t>
+  </si>
+  <si>
+    <t>Forward Looking</t>
+  </si>
+  <si>
+    <t>Sales Down 10-20%. Price up 1.5%.</t>
+  </si>
+  <si>
+    <t>Sales Down 10-15%. Price up 1.0%.</t>
+  </si>
+  <si>
+    <t>Sales down 10%. Price up 1.5%.</t>
+  </si>
+  <si>
+    <t>US &amp; Canada, Large Ag</t>
+  </si>
+  <si>
+    <t>Down 10-15%.</t>
+  </si>
+  <si>
+    <t>US &amp; Canada, Small Ag &amp; Turf</t>
+  </si>
+  <si>
+    <t>Down 5-10%.</t>
+  </si>
+  <si>
+    <t>Europe Ag &amp; Turf</t>
+  </si>
+  <si>
+    <t>Down 10%.</t>
+  </si>
+  <si>
+    <t>South America Tractors &amp; Combines</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Down moderately.</t>
+  </si>
+  <si>
+    <t>US &amp; Canada, Construction</t>
+  </si>
+  <si>
+    <t>US &amp; Canada, Compact Construction</t>
+  </si>
+  <si>
+    <t>Flat to down 5%.</t>
+  </si>
+  <si>
+    <t>Global Forestry</t>
+  </si>
+  <si>
+    <t>Global Roadbuilding</t>
+  </si>
+  <si>
+    <t>Flat.</t>
+  </si>
+  <si>
+    <t>Financial Services</t>
+  </si>
+  <si>
+    <t>Net income roughly $770.</t>
+  </si>
 </sst>
 </file>
 
@@ -950,7 +1025,7 @@
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1033,8 +1108,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1423,7 +1496,7 @@
   <dimension ref="B2:L23"/>
   <sheetViews>
     <sheetView zoomScale="135" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -1621,9 +1694,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858921DB-62EE-49E5-94B1-0F56666D22CA}">
   <dimension ref="A1:XFA111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G25" sqref="G25"/>
+      <selection pane="topRight" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1633,7 +1706,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16381">
-      <c r="E1" s="56">
+      <c r="E1" s="54">
         <v>45229</v>
       </c>
     </row>
@@ -18799,7 +18872,7 @@
       <c r="K27" s="49"/>
       <c r="L27" s="49"/>
       <c r="M27" s="49">
-        <f t="shared" ref="K27:N27" si="9">SUM(M24:M26)</f>
+        <f t="shared" ref="M27:N27" si="9">SUM(M24:M26)</f>
         <v>61252</v>
       </c>
       <c r="N27" s="49">
@@ -18879,7 +18952,7 @@
       <c r="K29" s="49"/>
       <c r="L29" s="49"/>
       <c r="M29" s="49">
-        <f t="shared" ref="K29:N29" si="11">M27-M28</f>
+        <f t="shared" ref="M29:N29" si="11">M27-M28</f>
         <v>23537</v>
       </c>
       <c r="N29" s="49">
@@ -18922,32 +18995,32 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="50" customFormat="1">
-      <c r="A31" s="50" t="s">
+    <row r="31" spans="1:14">
+      <c r="A31" t="s">
         <v>174</v>
       </c>
-      <c r="B31" s="51">
+      <c r="B31" s="48">
         <v>952</v>
       </c>
-      <c r="C31" s="51">
+      <c r="C31" s="48">
         <v>1330</v>
       </c>
-      <c r="D31" s="51">
+      <c r="D31" s="48">
         <v>1110</v>
       </c>
-      <c r="E31" s="51">
+      <c r="E31" s="48">
         <v>1203</v>
       </c>
-      <c r="F31" s="51">
+      <c r="F31" s="48">
         <v>1066</v>
       </c>
-      <c r="G31" s="51">
+      <c r="G31" s="48">
         <v>1265</v>
       </c>
-      <c r="H31" s="51">
+      <c r="H31" s="48">
         <v>1278</v>
       </c>
-      <c r="I31" s="51"/>
+      <c r="I31" s="48"/>
       <c r="K31" s="49"/>
       <c r="L31" s="49"/>
       <c r="M31" s="48">
@@ -18960,7 +19033,7 @@
       </c>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="50" t="s">
+      <c r="A32" t="s">
         <v>175</v>
       </c>
       <c r="B32" s="48">
@@ -18995,7 +19068,7 @@
       </c>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="50" t="s">
+      <c r="A33" t="s">
         <v>176</v>
       </c>
       <c r="B33" s="48">
@@ -19067,7 +19140,7 @@
       <c r="K34" s="49"/>
       <c r="L34" s="49"/>
       <c r="M34" s="49">
-        <f t="shared" ref="K34:N34" si="13">SUM(M30:M33)+M28</f>
+        <f t="shared" ref="M34:N34" si="13">SUM(M30:M33)+M28</f>
         <v>48232</v>
       </c>
       <c r="N34" s="49">
@@ -19111,7 +19184,7 @@
       <c r="K35" s="49"/>
       <c r="L35" s="49"/>
       <c r="M35" s="49">
-        <f t="shared" ref="K35:N35" si="15">M27-M34</f>
+        <f t="shared" ref="M35:N35" si="15">M27-M34</f>
         <v>13020</v>
       </c>
       <c r="N35" s="49">
@@ -19192,7 +19265,7 @@
       <c r="K37" s="49"/>
       <c r="L37" s="49"/>
       <c r="M37" s="49">
-        <f t="shared" ref="K37:N37" si="17">M35-M36</f>
+        <f t="shared" ref="M37:N37" si="17">M35-M36</f>
         <v>10149</v>
       </c>
       <c r="N37" s="49">
@@ -19304,7 +19377,7 @@
       <c r="K40" s="49"/>
       <c r="L40" s="49"/>
       <c r="M40" s="49">
-        <f t="shared" ref="K40:N40" si="19">M37+M38-M39</f>
+        <f t="shared" ref="M40:N40" si="19">M37+M38-M39</f>
         <v>10166</v>
       </c>
       <c r="N40" s="49">
@@ -19321,42 +19394,42 @@
       <c r="A43" s="47" t="s">
         <v>184</v>
       </c>
-      <c r="B43" s="55">
+      <c r="B43" s="53">
         <f t="shared" ref="B43:G43" si="20">B40/B49</f>
         <v>6.5826612903225801</v>
       </c>
-      <c r="C43" s="55">
+      <c r="C43" s="53">
         <f t="shared" si="20"/>
         <v>9.6916299559471355</v>
       </c>
-      <c r="D43" s="55">
+      <c r="D43" s="53">
         <f t="shared" si="20"/>
         <v>10.240715268225584</v>
       </c>
-      <c r="E43" s="55">
+      <c r="E43" s="53">
         <f t="shared" si="20"/>
         <v>8.2977232924693514</v>
       </c>
-      <c r="F43" s="55">
+      <c r="F43" s="53">
         <f t="shared" si="20"/>
         <v>6.2558056448731696</v>
       </c>
-      <c r="G43" s="55">
+      <c r="G43" s="53">
         <f t="shared" si="20"/>
         <v>8.5621387283236992</v>
       </c>
-      <c r="H43" s="55">
+      <c r="H43" s="53">
         <f>H40/H49</f>
         <v>6.3169398907103824</v>
       </c>
-      <c r="I43" s="55"/>
-      <c r="K43" s="55"/>
-      <c r="L43" s="55"/>
-      <c r="M43" s="55">
-        <f t="shared" ref="K43:N43" si="21">M40/M49</f>
+      <c r="I43" s="53"/>
+      <c r="K43" s="53"/>
+      <c r="L43" s="53"/>
+      <c r="M43" s="53">
+        <f t="shared" ref="M43:N43" si="21">M40/M49</f>
         <v>34.791238877481177</v>
       </c>
-      <c r="N43" s="55" t="e">
+      <c r="N43" s="53" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
@@ -19365,42 +19438,42 @@
       <c r="A44" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="B44" s="55">
+      <c r="B44" s="53">
         <f t="shared" ref="B44:G44" si="22">B40/B50</f>
         <v>6.549648946840521</v>
       </c>
-      <c r="C44" s="55">
+      <c r="C44" s="53">
         <f t="shared" si="22"/>
         <v>9.6458684654300164</v>
       </c>
-      <c r="D44" s="55">
+      <c r="D44" s="53">
         <f t="shared" si="22"/>
         <v>10.195138651146866</v>
       </c>
-      <c r="E44" s="55">
+      <c r="E44" s="53">
         <f t="shared" si="22"/>
         <v>8.257232485186476</v>
       </c>
-      <c r="F44" s="55">
+      <c r="F44" s="53">
         <f t="shared" si="22"/>
         <v>6.2290999644254708</v>
       </c>
-      <c r="G44" s="55">
+      <c r="G44" s="53">
         <f t="shared" si="22"/>
         <v>8.5282475710687304</v>
       </c>
-      <c r="H44" s="55">
+      <c r="H44" s="53">
         <f>H40/H50</f>
         <v>6.3146394756008739</v>
       </c>
-      <c r="I44" s="55"/>
-      <c r="K44" s="55"/>
-      <c r="L44" s="55"/>
-      <c r="M44" s="55">
-        <f t="shared" ref="K44:N44" si="23">M40/M50</f>
+      <c r="I44" s="53"/>
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="53">
+        <f t="shared" ref="M44:N44" si="23">M40/M50</f>
         <v>34.625340599455036</v>
       </c>
-      <c r="N44" s="55" t="e">
+      <c r="N44" s="53" t="e">
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
@@ -19409,34 +19482,34 @@
       <c r="A45" t="s">
         <v>186</v>
       </c>
-      <c r="B45" s="53">
+      <c r="B45" s="51">
         <v>1.2</v>
       </c>
-      <c r="C45" s="53">
+      <c r="C45" s="51">
         <v>1.25</v>
       </c>
-      <c r="D45" s="53">
+      <c r="D45" s="51">
         <v>1.25</v>
       </c>
-      <c r="E45" s="53">
+      <c r="E45" s="51">
         <v>1.35</v>
       </c>
-      <c r="F45" s="53">
+      <c r="F45" s="51">
         <v>1.47</v>
       </c>
-      <c r="G45" s="53">
+      <c r="G45" s="51">
         <v>1.47</v>
       </c>
-      <c r="H45" s="53">
+      <c r="H45" s="51">
         <v>1.47</v>
       </c>
-      <c r="I45" s="53"/>
+      <c r="I45" s="51"/>
       <c r="L45" s="47"/>
-      <c r="M45" s="53">
+      <c r="M45" s="51">
         <f t="shared" ref="M45:N46" si="24">SUM(B45:E45)</f>
         <v>5.0500000000000007</v>
       </c>
-      <c r="N45" s="53">
+      <c r="N45" s="51">
         <f t="shared" si="24"/>
         <v>5.32</v>
       </c>
@@ -19445,86 +19518,86 @@
       <c r="A46" t="s">
         <v>187</v>
       </c>
-      <c r="B46" s="53">
+      <c r="B46" s="51">
         <v>1.1299999999999999</v>
       </c>
-      <c r="C46" s="53">
+      <c r="C46" s="51">
         <v>1.2</v>
       </c>
-      <c r="D46" s="53">
+      <c r="D46" s="51">
         <v>1.25</v>
       </c>
-      <c r="E46" s="53">
+      <c r="E46" s="51">
         <v>1.25</v>
       </c>
-      <c r="F46" s="53">
+      <c r="F46" s="51">
         <v>1.35</v>
       </c>
-      <c r="G46" s="53">
+      <c r="G46" s="51">
         <v>1.47</v>
       </c>
-      <c r="H46" s="53">
+      <c r="H46" s="51">
         <v>1.47</v>
       </c>
-      <c r="I46" s="53"/>
-      <c r="M46" s="53">
+      <c r="I46" s="51"/>
+      <c r="M46" s="51">
         <f t="shared" si="24"/>
         <v>4.83</v>
       </c>
-      <c r="N46" s="53">
+      <c r="N46" s="51">
         <f t="shared" si="24"/>
         <v>5.0500000000000007</v>
       </c>
     </row>
     <row r="47" spans="1:14">
-      <c r="B47" s="52"/>
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="52"/>
-      <c r="F47" s="52"/>
-      <c r="G47" s="52"/>
-      <c r="H47" s="52"/>
-      <c r="I47" s="52"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
     </row>
     <row r="48" spans="1:14" s="47" customFormat="1">
       <c r="A48" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="B48" s="54"/>
-      <c r="C48" s="54"/>
-      <c r="D48" s="54"/>
-      <c r="E48" s="54"/>
-      <c r="F48" s="54"/>
-      <c r="G48" s="54"/>
-      <c r="H48" s="54"/>
-      <c r="I48" s="54"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="52"/>
+      <c r="H48" s="52"/>
+      <c r="I48" s="52"/>
     </row>
     <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>184</v>
       </c>
-      <c r="B49" s="52">
+      <c r="B49" s="50">
         <v>297.60000000000002</v>
       </c>
-      <c r="C49" s="52">
+      <c r="C49" s="50">
         <v>295.10000000000002</v>
       </c>
-      <c r="D49" s="52">
+      <c r="D49" s="50">
         <v>290.8</v>
       </c>
-      <c r="E49" s="52">
+      <c r="E49" s="50">
         <v>285.5</v>
       </c>
-      <c r="F49" s="52">
+      <c r="F49" s="50">
         <v>279.89999999999998</v>
       </c>
-      <c r="G49" s="52">
+      <c r="G49" s="50">
         <v>276.8</v>
       </c>
-      <c r="H49" s="52">
+      <c r="H49" s="50">
         <v>274.5</v>
       </c>
-      <c r="I49" s="52"/>
+      <c r="I49" s="50"/>
       <c r="M49">
         <v>292.2</v>
       </c>
@@ -19533,67 +19606,67 @@
       <c r="A50" t="s">
         <v>185</v>
       </c>
-      <c r="B50" s="52">
+      <c r="B50" s="50">
         <v>299.10000000000002</v>
       </c>
-      <c r="C50" s="52">
+      <c r="C50" s="50">
         <v>296.5</v>
       </c>
-      <c r="D50" s="52">
+      <c r="D50" s="50">
         <v>292.10000000000002</v>
       </c>
-      <c r="E50" s="52">
+      <c r="E50" s="50">
         <v>286.89999999999998</v>
       </c>
-      <c r="F50" s="52">
+      <c r="F50" s="50">
         <v>281.10000000000002</v>
       </c>
-      <c r="G50" s="52">
+      <c r="G50" s="50">
         <v>277.89999999999998</v>
       </c>
-      <c r="H50" s="52">
+      <c r="H50" s="50">
         <v>274.60000000000002</v>
       </c>
-      <c r="I50" s="52"/>
+      <c r="I50" s="50"/>
       <c r="M50">
         <v>293.60000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:14" s="50" customFormat="1">
+    <row r="52" spans="1:14">
       <c r="A52" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B52" s="51">
+      <c r="B52" s="48">
         <v>1957</v>
       </c>
-      <c r="C52" s="51">
+      <c r="C52" s="48">
         <f>4815-B52</f>
         <v>2858</v>
       </c>
-      <c r="D52" s="51">
+      <c r="D52" s="48">
         <f>7787-C52-B52</f>
         <v>2972</v>
       </c>
-      <c r="E52" s="51">
+      <c r="E52" s="48">
         <f>M52-D52-C52-B52</f>
         <v>2368</v>
       </c>
-      <c r="F52" s="51">
+      <c r="F52" s="48">
         <v>1748</v>
       </c>
-      <c r="G52" s="51">
+      <c r="G52" s="48">
         <f>4116-F52</f>
         <v>2368</v>
       </c>
-      <c r="H52" s="51">
+      <c r="H52" s="48">
         <f>5846-G52-F52</f>
         <v>1730</v>
       </c>
-      <c r="I52" s="51"/>
-      <c r="M52" s="51">
+      <c r="I52" s="48"/>
+      <c r="M52" s="48">
         <v>10155</v>
       </c>
-      <c r="N52" s="51"/>
+      <c r="N52" s="48"/>
     </row>
     <row r="53" spans="1:14">
       <c r="A53" s="14" t="s">
@@ -19610,7 +19683,7 @@
         <f>-64-C53-B53</f>
         <v>25</v>
       </c>
-      <c r="E53" s="51">
+      <c r="E53" s="48">
         <f t="shared" ref="E53:E63" si="25">M53-D53-C53-B53</f>
         <v>48</v>
       </c>
@@ -19621,11 +19694,11 @@
         <f>131-F53</f>
         <v>100</v>
       </c>
-      <c r="H53" s="51">
+      <c r="H53" s="48">
         <f>222-G53-F53</f>
         <v>91</v>
       </c>
-      <c r="I53" s="51"/>
+      <c r="I53" s="48"/>
       <c r="M53" s="48">
         <v>-16</v>
       </c>
@@ -19646,7 +19719,7 @@
         <f>1527-C54-B54</f>
         <v>532</v>
       </c>
-      <c r="E54" s="51">
+      <c r="E54" s="48">
         <f t="shared" si="25"/>
         <v>477</v>
       </c>
@@ -19657,11 +19730,11 @@
         <f>1045-F54</f>
         <v>525</v>
       </c>
-      <c r="H54" s="51">
+      <c r="H54" s="48">
         <f>1598-G54-F54</f>
         <v>553</v>
       </c>
-      <c r="I54" s="51"/>
+      <c r="I54" s="48"/>
       <c r="M54" s="48">
         <v>2004</v>
       </c>
@@ -19680,15 +19753,15 @@
       <c r="D55" s="48">
         <v>0</v>
       </c>
-      <c r="E55" s="51">
+      <c r="E55" s="48">
         <f t="shared" si="25"/>
         <v>18</v>
       </c>
-      <c r="H55" s="51">
+      <c r="H55" s="48">
         <f>53-G55-F55</f>
         <v>53</v>
       </c>
-      <c r="I55" s="51"/>
+      <c r="I55" s="48"/>
       <c r="M55" s="48">
         <v>191</v>
       </c>
@@ -19709,7 +19782,7 @@
         <f>112-C56-B56</f>
         <v>58</v>
       </c>
-      <c r="E56" s="51">
+      <c r="E56" s="48">
         <f t="shared" si="25"/>
         <v>18</v>
       </c>
@@ -19720,11 +19793,11 @@
         <f>104-F56</f>
         <v>58</v>
       </c>
-      <c r="H56" s="51">
+      <c r="H56" s="48">
         <f>159-G56-F56</f>
         <v>55</v>
       </c>
-      <c r="I56" s="51"/>
+      <c r="I56" s="48"/>
       <c r="M56" s="48">
         <v>130</v>
       </c>
@@ -19745,7 +19818,7 @@
         <f>-429-C57-B57</f>
         <v>-52</v>
       </c>
-      <c r="E57" s="51">
+      <c r="E57" s="48">
         <f t="shared" si="25"/>
         <v>-361</v>
       </c>
@@ -19756,11 +19829,11 @@
         <f>-120-F57</f>
         <v>-147</v>
       </c>
-      <c r="H57" s="51">
+      <c r="H57" s="48">
         <f>-125-G57-F57</f>
         <v>-5</v>
       </c>
-      <c r="I57" s="51"/>
+      <c r="I57" s="48"/>
       <c r="M57" s="48">
         <v>-790</v>
       </c>
@@ -19781,7 +19854,7 @@
         <f>-5059-C58-B58</f>
         <v>-652</v>
       </c>
-      <c r="E58" s="51">
+      <c r="E58" s="48">
         <f t="shared" si="25"/>
         <v>806</v>
       </c>
@@ -19792,11 +19865,11 @@
         <f>-2469-F58</f>
         <v>-2192</v>
       </c>
-      <c r="H58" s="51">
+      <c r="H58" s="48">
         <f>-2446-G58-F58</f>
         <v>23</v>
       </c>
-      <c r="I58" s="51"/>
+      <c r="I58" s="48"/>
       <c r="M58" s="48">
         <v>-4253</v>
       </c>
@@ -19817,7 +19890,7 @@
         <f>-663-C59-B59</f>
         <v>319</v>
       </c>
-      <c r="E59" s="51">
+      <c r="E59" s="48">
         <f t="shared" si="25"/>
         <v>942</v>
       </c>
@@ -19828,11 +19901,11 @@
         <f>-409-F59</f>
         <v>314</v>
       </c>
-      <c r="H59" s="51">
+      <c r="H59" s="48">
         <f>234-G59-F59</f>
         <v>643</v>
       </c>
-      <c r="I59" s="51"/>
+      <c r="I59" s="48"/>
       <c r="M59" s="48">
         <v>279</v>
       </c>
@@ -19853,7 +19926,7 @@
         <f>47-C60-B60</f>
         <v>360</v>
       </c>
-      <c r="E60" s="51">
+      <c r="E60" s="48">
         <f t="shared" si="25"/>
         <v>783</v>
       </c>
@@ -19864,11 +19937,11 @@
         <f>-1300-F60</f>
         <v>1027</v>
       </c>
-      <c r="H60" s="51">
+      <c r="H60" s="48">
         <f>-1015-G60-F60</f>
         <v>285</v>
       </c>
-      <c r="I60" s="51"/>
+      <c r="I60" s="48"/>
       <c r="M60" s="48">
         <v>830</v>
       </c>
@@ -19889,7 +19962,7 @@
         <f>-595-C61-B61</f>
         <v>-499</v>
       </c>
-      <c r="E61" s="51">
+      <c r="E61" s="48">
         <f t="shared" si="25"/>
         <v>572</v>
       </c>
@@ -19900,11 +19973,11 @@
         <f>-29-F61</f>
         <v>-212</v>
       </c>
-      <c r="H61" s="51">
+      <c r="H61" s="48">
         <f>31-G61-F61</f>
         <v>60</v>
       </c>
-      <c r="I61" s="51"/>
+      <c r="I61" s="48"/>
       <c r="M61" s="48">
         <v>-23</v>
       </c>
@@ -19925,7 +19998,7 @@
         <f>-116-C62-B62</f>
         <v>-48</v>
       </c>
-      <c r="E62" s="51">
+      <c r="E62" s="48">
         <f t="shared" si="25"/>
         <v>-54</v>
       </c>
@@ -19936,11 +20009,11 @@
         <f>-208-F62</f>
         <v>-79</v>
       </c>
-      <c r="H62" s="51">
+      <c r="H62" s="48">
         <f>-246-G62-F62</f>
         <v>-38</v>
       </c>
-      <c r="I62" s="51"/>
+      <c r="I62" s="48"/>
       <c r="M62" s="48">
         <v>-170</v>
       </c>
@@ -19961,7 +20034,7 @@
         <f>176-C63-B63</f>
         <v>28</v>
       </c>
-      <c r="E63" s="51">
+      <c r="E63" s="48">
         <f t="shared" si="25"/>
         <v>76</v>
       </c>
@@ -19972,11 +20045,11 @@
         <f>83-F63</f>
         <v>90</v>
       </c>
-      <c r="H63" s="51">
+      <c r="H63" s="48">
         <f>-172-G63-F63</f>
         <v>-255</v>
       </c>
-      <c r="I63" s="51"/>
+      <c r="I63" s="48"/>
       <c r="M63" s="48">
         <v>252</v>
       </c>
@@ -19987,40 +20060,40 @@
         <v>20</v>
       </c>
       <c r="B64" s="49">
-        <f>SUM(B52:B63)</f>
+        <f t="shared" ref="B64:H64" si="26">SUM(B52:B63)</f>
         <v>-1246</v>
       </c>
       <c r="C64" s="49">
-        <f>SUM(C52:C63)</f>
+        <f t="shared" si="26"/>
         <v>1099</v>
       </c>
       <c r="D64" s="49">
-        <f>SUM(D52:D63)</f>
+        <f t="shared" si="26"/>
         <v>3043</v>
       </c>
       <c r="E64" s="49">
-        <f>SUM(E52:E63)</f>
+        <f t="shared" si="26"/>
         <v>5693</v>
       </c>
       <c r="F64" s="49">
-        <f>SUM(F52:F63)</f>
+        <f t="shared" si="26"/>
         <v>-908</v>
       </c>
       <c r="G64" s="49">
-        <f>SUM(G52:G63)</f>
+        <f t="shared" si="26"/>
         <v>1852</v>
       </c>
       <c r="H64" s="49">
-        <f>SUM(H52:H63)</f>
+        <f t="shared" si="26"/>
         <v>3195</v>
       </c>
       <c r="I64" s="49"/>
       <c r="M64" s="49">
-        <f t="shared" ref="M64:N64" si="26">SUM(M52:M63)</f>
+        <f t="shared" ref="M64:N64" si="27">SUM(M52:M63)</f>
         <v>8589</v>
       </c>
       <c r="N64" s="49">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -20029,11 +20102,11 @@
     </row>
     <row r="66" spans="1:14" s="47" customFormat="1">
       <c r="B66" s="47" t="str">
-        <f t="shared" ref="B66:C66" si="27">B22</f>
+        <f t="shared" ref="B66:C66" si="28">B22</f>
         <v>Q123</v>
       </c>
       <c r="C66" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>Q223</v>
       </c>
       <c r="D66" s="47" t="str">
@@ -20041,15 +20114,15 @@
         <v>Q323</v>
       </c>
       <c r="E66" s="47" t="str">
-        <f t="shared" ref="E66:G66" si="28">E22</f>
+        <f t="shared" ref="E66:G66" si="29">E22</f>
         <v>Q423</v>
       </c>
       <c r="F66" s="47" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Q124</v>
       </c>
       <c r="G66" s="47" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Q224</v>
       </c>
       <c r="H66" s="47" t="str">
@@ -20128,7 +20201,7 @@
       </c>
       <c r="I69" s="48"/>
       <c r="M69" s="48">
-        <f t="shared" ref="M69:M75" si="29">E69</f>
+        <f t="shared" ref="M69:M75" si="30">E69</f>
         <v>946</v>
       </c>
     </row>
@@ -20159,7 +20232,7 @@
       </c>
       <c r="I70" s="48"/>
       <c r="M70" s="48">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>7739</v>
       </c>
     </row>
@@ -20190,7 +20263,7 @@
       </c>
       <c r="I71" s="48"/>
       <c r="M71" s="48">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>43673</v>
       </c>
     </row>
@@ -20221,7 +20294,7 @@
       </c>
       <c r="I72" s="48"/>
       <c r="M72" s="48">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>7335</v>
       </c>
     </row>
@@ -20252,7 +20325,7 @@
       </c>
       <c r="I73" s="48"/>
       <c r="M73" s="48">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2623</v>
       </c>
     </row>
@@ -20283,7 +20356,7 @@
       </c>
       <c r="I74" s="48"/>
       <c r="M74" s="48">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>6917</v>
       </c>
     </row>
@@ -20314,7 +20387,7 @@
       </c>
       <c r="I75" s="48"/>
       <c r="M75" s="48">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>8160</v>
       </c>
     </row>
@@ -20323,27 +20396,27 @@
         <v>195</v>
       </c>
       <c r="B76" s="49">
-        <f t="shared" ref="B76:G76" si="30">SUM(B67:B75)</f>
+        <f t="shared" ref="B76:G76" si="31">SUM(B67:B75)</f>
         <v>72958</v>
       </c>
       <c r="C76" s="49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>79537</v>
       </c>
       <c r="D76" s="49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>84194</v>
       </c>
       <c r="E76" s="49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>84851</v>
       </c>
       <c r="F76" s="49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>81881</v>
       </c>
       <c r="G76" s="49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>86010</v>
       </c>
       <c r="H76" s="49">
@@ -20383,7 +20456,7 @@
       </c>
       <c r="I77" s="48"/>
       <c r="M77" s="48">
-        <f t="shared" ref="M77:M83" si="31">E77</f>
+        <f t="shared" ref="M77:M83" si="32">E77</f>
         <v>6879</v>
       </c>
     </row>
@@ -20414,7 +20487,7 @@
       </c>
       <c r="I78" s="48"/>
       <c r="M78" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>3900</v>
       </c>
     </row>
@@ -20445,7 +20518,7 @@
       </c>
       <c r="I79" s="48"/>
       <c r="M79" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1133</v>
       </c>
     </row>
@@ -20476,7 +20549,7 @@
       </c>
       <c r="I80" s="48"/>
       <c r="M80" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>3007</v>
       </c>
     </row>
@@ -20507,7 +20580,7 @@
       </c>
       <c r="I81" s="48"/>
       <c r="M81" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1814</v>
       </c>
     </row>
@@ -20538,7 +20611,7 @@
       </c>
       <c r="I82" s="48"/>
       <c r="M82" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2503</v>
       </c>
     </row>
@@ -20569,7 +20642,7 @@
       </c>
       <c r="I83" s="48"/>
       <c r="M83" s="48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -20578,36 +20651,36 @@
         <v>201</v>
       </c>
       <c r="B84" s="49">
-        <f t="shared" ref="B84:H84" si="32">SUM(B76:B83)</f>
+        <f t="shared" ref="B84:H84" si="33">SUM(B76:B83)</f>
         <v>91620</v>
       </c>
       <c r="C84" s="49">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>98347</v>
       </c>
       <c r="D84" s="49">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>103397</v>
       </c>
       <c r="E84" s="49">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>104087</v>
       </c>
       <c r="F84" s="49">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>101371</v>
       </c>
       <c r="G84" s="49">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>105628</v>
       </c>
       <c r="H84" s="49">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>107841</v>
       </c>
       <c r="I84" s="49"/>
       <c r="M84" s="49">
-        <f t="shared" ref="M84" si="33">SUM(M76:M83)</f>
+        <f t="shared" ref="M84" si="34">SUM(M76:M83)</f>
         <v>104087</v>
       </c>
     </row>
@@ -20643,43 +20716,43 @@
       </c>
       <c r="I87" s="48"/>
       <c r="M87" s="48">
-        <f t="shared" ref="M87:M97" si="34">E87</f>
+        <f t="shared" ref="M87:M97" si="35">E87</f>
         <v>17939</v>
       </c>
     </row>
-    <row r="88" spans="1:13" s="50" customFormat="1">
-      <c r="A88" s="50" t="s">
+    <row r="88" spans="1:13">
+      <c r="A88" t="s">
         <v>206</v>
       </c>
-      <c r="B88" s="51">
+      <c r="B88" s="48">
         <v>4864</v>
       </c>
-      <c r="C88" s="51">
+      <c r="C88" s="48">
         <v>5379</v>
       </c>
-      <c r="D88" s="51">
+      <c r="D88" s="48">
         <v>6608</v>
       </c>
-      <c r="E88" s="51">
+      <c r="E88" s="48">
         <v>6995</v>
       </c>
-      <c r="F88" s="51">
+      <c r="F88" s="48">
         <v>6116</v>
       </c>
-      <c r="G88" s="51">
+      <c r="G88" s="48">
         <v>6976</v>
       </c>
-      <c r="H88" s="51">
+      <c r="H88" s="48">
         <v>7869</v>
       </c>
-      <c r="I88" s="51"/>
+      <c r="I88" s="48"/>
       <c r="M88" s="48">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6995</v>
       </c>
     </row>
     <row r="89" spans="1:13">
-      <c r="A89" s="50" t="s">
+      <c r="A89" t="s">
         <v>207</v>
       </c>
       <c r="B89" s="48">
@@ -20705,12 +20778,12 @@
       </c>
       <c r="I89" s="48"/>
       <c r="M89" s="48">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>16130</v>
       </c>
     </row>
     <row r="90" spans="1:13">
-      <c r="A90" s="50" t="s">
+      <c r="A90" t="s">
         <v>199</v>
       </c>
       <c r="B90" s="48">
@@ -20736,7 +20809,7 @@
       </c>
       <c r="I90" s="48"/>
       <c r="M90" s="48">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>520</v>
       </c>
     </row>
@@ -20745,27 +20818,27 @@
         <v>211</v>
       </c>
       <c r="B91" s="49">
-        <f t="shared" ref="B91:G91" si="35">SUM(B87:B90)</f>
+        <f t="shared" ref="B91:G91" si="36">SUM(B87:B90)</f>
         <v>32620</v>
       </c>
       <c r="C91" s="49">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>37715</v>
       </c>
       <c r="D91" s="49">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>39597</v>
       </c>
       <c r="E91" s="49">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>41584</v>
       </c>
       <c r="F91" s="49">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>37144</v>
       </c>
       <c r="G91" s="49">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>39775</v>
       </c>
       <c r="H91" s="49">
@@ -20780,7 +20853,7 @@
       </c>
     </row>
     <row r="92" spans="1:13">
-      <c r="A92" s="50" t="s">
+      <c r="A92" t="s">
         <v>208</v>
       </c>
       <c r="B92" s="48">
@@ -20807,12 +20880,12 @@
       <c r="I92" s="48"/>
       <c r="J92" s="48"/>
       <c r="M92" s="48">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>38477</v>
       </c>
     </row>
     <row r="93" spans="1:13">
-      <c r="A93" s="50" t="s">
+      <c r="A93" t="s">
         <v>209</v>
       </c>
       <c r="B93" s="48">
@@ -20839,12 +20912,12 @@
       <c r="I93" s="48"/>
       <c r="J93" s="48"/>
       <c r="M93" s="48">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>2140</v>
       </c>
     </row>
     <row r="94" spans="1:13">
-      <c r="A94" s="50" t="s">
+      <c r="A94" t="s">
         <v>210</v>
       </c>
       <c r="B94" s="48">
@@ -20871,7 +20944,7 @@
       <c r="I94" s="48"/>
       <c r="J94" s="48"/>
       <c r="M94" s="48">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
     </row>
@@ -20880,27 +20953,27 @@
         <v>212</v>
       </c>
       <c r="B95" s="49">
-        <f t="shared" ref="B95:G95" si="36">SUM(B91:B94)</f>
+        <f t="shared" ref="B95:G95" si="37">SUM(B91:B94)</f>
         <v>70184</v>
       </c>
       <c r="C95" s="49">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>75846</v>
       </c>
       <c r="D95" s="49">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>80245</v>
       </c>
       <c r="E95" s="49">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>82201</v>
       </c>
       <c r="F95" s="49">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>79192</v>
       </c>
       <c r="G95" s="49">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>82842</v>
       </c>
       <c r="H95" s="49">
@@ -20914,41 +20987,41 @@
         <v>82201</v>
       </c>
     </row>
-    <row r="96" spans="1:13" s="50" customFormat="1">
-      <c r="A96" s="50" t="s">
+    <row r="96" spans="1:13">
+      <c r="A96" t="s">
         <v>215</v>
       </c>
-      <c r="B96" s="51">
+      <c r="B96" s="48">
         <v>100</v>
       </c>
-      <c r="C96" s="51">
+      <c r="C96" s="48">
         <v>102</v>
       </c>
-      <c r="D96" s="51">
+      <c r="D96" s="48">
         <v>101</v>
       </c>
-      <c r="E96" s="51">
+      <c r="E96" s="48">
         <v>97</v>
       </c>
-      <c r="F96" s="51">
+      <c r="F96" s="48">
         <v>100</v>
       </c>
-      <c r="G96" s="51">
+      <c r="G96" s="48">
         <v>98</v>
       </c>
-      <c r="H96" s="51">
+      <c r="H96" s="48">
         <v>84</v>
       </c>
-      <c r="I96" s="51"/>
-      <c r="J96" s="51"/>
+      <c r="I96" s="48"/>
+      <c r="J96" s="48"/>
       <c r="M96" s="48">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>97</v>
       </c>
     </row>
     <row r="97" spans="1:13">
       <c r="M97" s="48">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
     </row>
@@ -20957,27 +21030,27 @@
         <v>213</v>
       </c>
       <c r="B98" s="49">
-        <f t="shared" ref="B98:G98" si="37">B84-B95-B96</f>
+        <f t="shared" ref="B98:G98" si="38">B84-B95-B96</f>
         <v>21336</v>
       </c>
       <c r="C98" s="49">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>22399</v>
       </c>
       <c r="D98" s="49">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>23051</v>
       </c>
       <c r="E98" s="49">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>21789</v>
       </c>
       <c r="F98" s="49">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>22079</v>
       </c>
       <c r="G98" s="49">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>22688</v>
       </c>
       <c r="H98" s="49">
@@ -21021,7 +21094,7 @@
         <v>5441</v>
       </c>
       <c r="M100" s="48">
-        <f t="shared" ref="M100:M103" si="38">E100</f>
+        <f t="shared" ref="M100:M103" si="39">E100</f>
         <v>5303</v>
       </c>
     </row>
@@ -21051,7 +21124,7 @@
         <v>-34570</v>
       </c>
       <c r="M101" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>-31335</v>
       </c>
     </row>
@@ -21081,7 +21154,7 @@
         <v>55559</v>
       </c>
       <c r="M102" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>50931</v>
       </c>
     </row>
@@ -21111,7 +21184,7 @@
         <v>-3368</v>
       </c>
       <c r="M103" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>-3114</v>
       </c>
     </row>
@@ -21120,27 +21193,27 @@
         <v>220</v>
       </c>
       <c r="B104" s="49">
-        <f t="shared" ref="B104:G104" si="39">SUM(B100:B103)</f>
+        <f t="shared" ref="B104:G104" si="40">SUM(B100:B103)</f>
         <v>21332</v>
       </c>
       <c r="C104" s="49">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>22395</v>
       </c>
       <c r="D104" s="49">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>23048</v>
       </c>
       <c r="E104" s="49">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>21785</v>
       </c>
       <c r="F104" s="49">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>22075</v>
       </c>
       <c r="G104" s="49">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>22684</v>
       </c>
       <c r="H104" s="49">
@@ -21178,7 +21251,7 @@
         <v>3</v>
       </c>
       <c r="M105" s="48">
-        <f t="shared" ref="M105" si="40">E105</f>
+        <f t="shared" ref="M105" si="41">E105</f>
         <v>4</v>
       </c>
     </row>
@@ -21187,27 +21260,27 @@
         <v>222</v>
       </c>
       <c r="B106" s="49">
-        <f t="shared" ref="B106:G106" si="41">B105+B104</f>
+        <f t="shared" ref="B106:G106" si="42">B105+B104</f>
         <v>21336</v>
       </c>
       <c r="C106" s="49">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>22399</v>
       </c>
       <c r="D106" s="49">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>23051</v>
       </c>
       <c r="E106" s="49">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>21789</v>
       </c>
       <c r="F106" s="49">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>22079</v>
       </c>
       <c r="G106" s="49">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>22688</v>
       </c>
       <c r="H106" s="49">
@@ -21228,32 +21301,32 @@
         <v>91620</v>
       </c>
       <c r="C107" s="49">
-        <f t="shared" ref="C107:H107" si="42">C106+C95+C96</f>
+        <f t="shared" ref="C107:H107" si="43">C106+C95+C96</f>
         <v>98347</v>
       </c>
       <c r="D107" s="49">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>103397</v>
       </c>
       <c r="E107" s="49">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>104087</v>
       </c>
       <c r="F107" s="49">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>101371</v>
       </c>
       <c r="G107" s="49">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>105628</v>
       </c>
       <c r="H107" s="49">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>107841</v>
       </c>
       <c r="I107" s="49"/>
       <c r="M107" s="49">
-        <f t="shared" ref="M107" si="43">M106+M95+M96</f>
+        <f t="shared" ref="M107" si="44">M106+M95+M96</f>
         <v>104087</v>
       </c>
     </row>
@@ -21261,37 +21334,37 @@
       <c r="A109" s="47" t="s">
         <v>224</v>
       </c>
-      <c r="B109" s="54">
-        <f t="shared" ref="B109:H109" si="44">B95/B84</f>
+      <c r="B109" s="52">
+        <f t="shared" ref="B109:H109" si="45">B95/B84</f>
         <v>0.76603361711416718</v>
       </c>
-      <c r="C109" s="54">
-        <f t="shared" si="44"/>
+      <c r="C109" s="52">
+        <f t="shared" si="45"/>
         <v>0.77120806938696651</v>
       </c>
-      <c r="D109" s="54">
-        <f t="shared" si="44"/>
+      <c r="D109" s="52">
+        <f t="shared" si="45"/>
         <v>0.77608634679923016</v>
       </c>
-      <c r="E109" s="54">
-        <f t="shared" si="44"/>
+      <c r="E109" s="52">
+        <f t="shared" si="45"/>
         <v>0.78973358824829232</v>
       </c>
-      <c r="F109" s="54">
-        <f t="shared" si="44"/>
+      <c r="F109" s="52">
+        <f t="shared" si="45"/>
         <v>0.78120961616241336</v>
       </c>
-      <c r="G109" s="54">
-        <f t="shared" si="44"/>
+      <c r="G109" s="52">
+        <f t="shared" si="45"/>
         <v>0.78428068315219446</v>
       </c>
-      <c r="H109" s="54">
-        <f t="shared" si="44"/>
+      <c r="H109" s="52">
+        <f t="shared" si="45"/>
         <v>0.7853413822201204</v>
       </c>
-      <c r="I109" s="54"/>
-      <c r="M109" s="54">
-        <f t="shared" ref="M109" si="45">M95/M84</f>
+      <c r="I109" s="52"/>
+      <c r="M109" s="52">
+        <f t="shared" ref="M109" si="46">M95/M84</f>
         <v>0.78973358824829232</v>
       </c>
     </row>
@@ -21299,36 +21372,36 @@
       <c r="A110" s="47" t="s">
         <v>225</v>
       </c>
-      <c r="B110" s="54">
-        <f t="shared" ref="B110:H110" si="46">B76/B91</f>
+      <c r="B110" s="52">
+        <f t="shared" ref="B110:G110" si="47">B76/B91</f>
         <v>2.2366033108522378</v>
       </c>
-      <c r="C110" s="54">
-        <f t="shared" si="46"/>
+      <c r="C110" s="52">
+        <f t="shared" si="47"/>
         <v>2.1088956648548325</v>
       </c>
-      <c r="D110" s="54">
-        <f t="shared" si="46"/>
+      <c r="D110" s="52">
+        <f t="shared" si="47"/>
         <v>2.1262721923378032</v>
       </c>
-      <c r="E110" s="54">
-        <f t="shared" si="46"/>
+      <c r="E110" s="52">
+        <f t="shared" si="47"/>
         <v>2.0404722970373221</v>
       </c>
-      <c r="F110" s="54">
-        <f t="shared" si="46"/>
+      <c r="F110" s="52">
+        <f t="shared" si="47"/>
         <v>2.2044206332112859</v>
       </c>
-      <c r="G110" s="54">
-        <f t="shared" si="46"/>
+      <c r="G110" s="52">
+        <f t="shared" si="47"/>
         <v>2.1624135763670647</v>
       </c>
-      <c r="H110" s="54">
+      <c r="H110" s="52">
         <f>H76/H91</f>
         <v>2.2309350437685653</v>
       </c>
-      <c r="I110" s="54"/>
-      <c r="M110" s="54">
+      <c r="I110" s="52"/>
+      <c r="M110" s="52">
         <f>M76/M91</f>
         <v>2.0404722970373221</v>
       </c>
@@ -21338,27 +21411,27 @@
         <v>226</v>
       </c>
       <c r="B111" s="49">
-        <f t="shared" ref="B111:H111" si="47">B76-B91</f>
+        <f t="shared" ref="B111:G111" si="48">B76-B91</f>
         <v>40338</v>
       </c>
       <c r="C111" s="49">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>41822</v>
       </c>
       <c r="D111" s="49">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>44597</v>
       </c>
       <c r="E111" s="49">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>43267</v>
       </c>
       <c r="F111" s="49">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>44737</v>
       </c>
       <c r="G111" s="49">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>46235</v>
       </c>
       <c r="H111" s="49">
@@ -25478,17 +25551,197 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF238C3A-91E4-4025-92B8-65E0C240F210}">
-  <dimension ref="B2"/>
+  <dimension ref="B2:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" t="s">
-        <v>54</v>
+    <row r="2" spans="2:5">
+      <c r="B2">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="C3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="C4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="C5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="C6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="C7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="C8" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" t="s">
+        <v>240</v>
+      </c>
+      <c r="E8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="C9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D9" t="s">
+        <v>242</v>
+      </c>
+      <c r="E9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="C10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="C11" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" t="s">
+        <v>245</v>
+      </c>
+      <c r="E11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="C12" t="s">
+        <v>234</v>
+      </c>
+      <c r="D12" t="s">
+        <v>247</v>
+      </c>
+      <c r="E12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="C13" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" t="s">
+        <v>248</v>
+      </c>
+      <c r="E13" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="C14" t="s">
+        <v>234</v>
+      </c>
+      <c r="D14" t="s">
+        <v>250</v>
+      </c>
+      <c r="E14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="C15" t="s">
+        <v>234</v>
+      </c>
+      <c r="D15" t="s">
+        <v>251</v>
+      </c>
+      <c r="E15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5">
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>231</v>
+      </c>
+      <c r="E18" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5">
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>232</v>
+      </c>
+      <c r="E19" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -25501,7 +25754,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>

</xml_diff>